<commit_message>
Fixed typos in AvTS § 35 lg 2 p 3 and STS2007_2013 § 25 lg 6
</commit_message>
<xml_diff>
--- a/htdocs/resources/Juurdepaasupiirangute_klassifikaator/v5/JPP_klassifikaator_alamklassifikaatoriga_201117_v_5_0.xlsx
+++ b/htdocs/resources/Juurdepaasupiirangute_klassifikaator/v5/JPP_klassifikaator_alamklassifikaatoriga_201117_v_5_0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Documents\Juhised\JPP klassifikaator\Versioon 5.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\filee\home\hannesk\My Documents\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -355,9 +355,6 @@
   </si>
   <si>
     <t>§ 25 lg 4</t>
-  </si>
-  <si>
-    <t>Omafinanseeringu allikad (v.a juhul kui need on saadud eelarvelistest vahenditest) ja hindamisse kaasatud isikute nimed hinnanguga seostatud kujul</t>
   </si>
   <si>
     <t>§ 25 lg 6</t>
@@ -1187,9 +1184,6 @@
     <t>Lennuõnnetuse uurimisorgani poolt kogutud teave </t>
   </si>
   <si>
-    <t>Põhjendatud juhtudel asutusesiseslt adresseeritud dokumendid</t>
-  </si>
-  <si>
     <t>Riigikontrolli hinnangud kontrolli tulemuste kohta enne kontrollaruande avalikustamist</t>
   </si>
   <si>
@@ -1358,11 +1352,17 @@
   <si>
     <t>Pakkumus on konfidentsiaalne</t>
   </si>
+  <si>
+    <t>Põhjendatud juhtudel asutusesiseselt adresseeritud dokumendid</t>
+  </si>
+  <si>
+    <t>Omafinantseeringu allikad (v.a juhul kui need on saadud eelarvelistest vahenditest) ja hindamisse kaasatud isikute nimed hinnanguga seostatud kujul</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="17">
     <font>
       <sz val="12"/>
@@ -1835,6 +1835,14 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1858,14 +1866,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -2258,8 +2258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H87" workbookViewId="0">
-      <selection activeCell="O92" sqref="O92"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2281,72 +2281,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="14" customFormat="1">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62" t="s">
-        <v>177</v>
-      </c>
-      <c r="C1" s="62" t="s">
-        <v>286</v>
-      </c>
-      <c r="D1" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="58" t="s">
+      <c r="B1" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="C1" s="66" t="s">
+        <v>284</v>
+      </c>
+      <c r="D1" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="59" t="s">
-        <v>213</v>
-      </c>
-      <c r="G1" s="58" t="s">
+      <c r="F1" s="63" t="s">
+        <v>212</v>
+      </c>
+      <c r="G1" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="58" t="s">
+      <c r="H1" s="62" t="s">
+        <v>172</v>
+      </c>
+      <c r="I1" s="62" t="s">
         <v>173</v>
       </c>
-      <c r="I1" s="58" t="s">
-        <v>174</v>
-      </c>
-      <c r="J1" s="64" t="s">
-        <v>290</v>
-      </c>
-      <c r="K1" s="65"/>
-      <c r="L1" s="64" t="s">
+      <c r="J1" s="68" t="s">
+        <v>288</v>
+      </c>
+      <c r="K1" s="69"/>
+      <c r="L1" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="65"/>
-      <c r="N1" s="58" t="s">
+      <c r="M1" s="69"/>
+      <c r="N1" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="58" t="s">
+      <c r="O1" s="62" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="14" customFormat="1">
-      <c r="A2" s="61"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
+      <c r="A2" s="65"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
       <c r="J2" s="15" t="s">
         <v>0</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L2" s="15" t="s">
         <v>0</v>
       </c>
       <c r="M2" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="N2" s="58"/>
-      <c r="O2" s="58"/>
+        <v>143</v>
+      </c>
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="18">
@@ -2360,7 +2360,7 @@
         <v>7</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="N3" s="16" t="s">
         <v>8</v>
@@ -2383,13 +2383,13 @@
         <v>9</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J4" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K4" s="16" t="s">
         <v>10</v>
@@ -2410,7 +2410,7 @@
         <v>11</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="N5" s="16" t="s">
         <v>8</v>
@@ -2434,22 +2434,22 @@
       </c>
       <c r="F6" s="24"/>
       <c r="G6" s="25" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J6" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K6" s="16" t="s">
         <v>10</v>
       </c>
       <c r="L6" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M6" s="29" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="N6" s="16" t="s">
         <v>8</v>
@@ -2467,7 +2467,7 @@
         <v>13</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N7" s="16" t="s">
         <v>8</v>
@@ -2490,19 +2490,19 @@
         <v>14</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K8" s="16" t="s">
         <v>10</v>
       </c>
       <c r="L8" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M8" s="30" t="s">
         <v>15</v>
@@ -2528,19 +2528,19 @@
         <v>16</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K9" s="16" t="s">
         <v>10</v>
       </c>
       <c r="L9" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M9" s="16" t="s">
         <v>15</v>
@@ -2566,13 +2566,13 @@
         <v>17</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K10" s="16" t="s">
         <v>10</v>
@@ -2598,13 +2598,13 @@
         <v>18</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K11" s="16" t="s">
         <v>10</v>
@@ -2630,13 +2630,13 @@
         <v>19</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K12" s="16" t="s">
         <v>10</v>
@@ -2662,13 +2662,13 @@
         <v>20</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K13" s="16" t="s">
         <v>10</v>
@@ -2697,13 +2697,13 @@
         <v>21</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J14" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K14" s="16" t="s">
         <v>10</v>
@@ -2729,13 +2729,13 @@
         <v>22</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J15" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K15" s="16" t="s">
         <v>10</v>
@@ -2759,16 +2759,16 @@
         <v>13</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G16" s="34" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J16" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K16" s="16" t="s">
         <v>10</v>
@@ -2792,16 +2792,16 @@
         <v>13</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G17" s="36" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="H17" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J17" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K17" s="16" t="s">
         <v>10</v>
@@ -2828,13 +2828,13 @@
         <v>23</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K18" s="16" t="s">
         <v>10</v>
@@ -2861,13 +2861,13 @@
         <v>24</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J19" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K19" s="16" t="s">
         <v>10</v>
@@ -2894,13 +2894,13 @@
         <v>25</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J20" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K20" s="16" t="s">
         <v>10</v>
@@ -2927,13 +2927,13 @@
         <v>26</v>
       </c>
       <c r="G21" s="23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J21" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K21" s="16" t="s">
         <v>10</v>
@@ -2963,13 +2963,13 @@
         <v>1</v>
       </c>
       <c r="G22" s="31" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J22" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K22" s="16" t="s">
         <v>10</v>
@@ -2999,16 +2999,16 @@
         <v>2</v>
       </c>
       <c r="G23" s="32" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K23" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N23" s="16" t="s">
         <v>8</v>
@@ -3035,16 +3035,16 @@
         <v>3</v>
       </c>
       <c r="G24" s="32" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H24" s="16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J24" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K24" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N24" s="16" t="s">
         <v>8</v>
@@ -3071,13 +3071,13 @@
         <v>1</v>
       </c>
       <c r="G25" s="32" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H25" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J25" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K25" s="16" t="s">
         <v>10</v>
@@ -3107,16 +3107,16 @@
         <v>2</v>
       </c>
       <c r="G26" s="32" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H26" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J26" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K26" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N26" s="16" t="s">
         <v>8</v>
@@ -3143,16 +3143,16 @@
         <v>3</v>
       </c>
       <c r="G27" s="32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H27" s="16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J27" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K27" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N27" s="16" t="s">
         <v>8</v>
@@ -3179,13 +3179,13 @@
         <v>1</v>
       </c>
       <c r="G28" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H28" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J28" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K28" s="16" t="s">
         <v>10</v>
@@ -3215,16 +3215,16 @@
         <v>2</v>
       </c>
       <c r="G29" s="32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H29" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J29" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K29" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N29" s="16" t="s">
         <v>8</v>
@@ -3251,16 +3251,16 @@
         <v>3</v>
       </c>
       <c r="G30" s="32" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H30" s="16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J30" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K30" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N30" s="16" t="s">
         <v>8</v>
@@ -3287,13 +3287,13 @@
         <v>1</v>
       </c>
       <c r="G31" s="32" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H31" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J31" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K31" s="16" t="s">
         <v>10</v>
@@ -3323,16 +3323,16 @@
         <v>2</v>
       </c>
       <c r="G32" s="32" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H32" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J32" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K32" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N32" s="16" t="s">
         <v>8</v>
@@ -3359,16 +3359,16 @@
         <v>3</v>
       </c>
       <c r="G33" s="32" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H33" s="16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J33" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K33" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N33" s="16" t="s">
         <v>8</v>
@@ -3395,13 +3395,13 @@
         <v>1</v>
       </c>
       <c r="G34" s="32" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H34" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J34" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K34" s="16" t="s">
         <v>10</v>
@@ -3431,16 +3431,16 @@
         <v>2</v>
       </c>
       <c r="G35" s="32" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H35" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J35" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K35" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N35" s="16" t="s">
         <v>8</v>
@@ -3467,16 +3467,16 @@
         <v>3</v>
       </c>
       <c r="G36" s="32" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H36" s="16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J36" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K36" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N36" s="16" t="s">
         <v>8</v>
@@ -3500,13 +3500,13 @@
         <v>32</v>
       </c>
       <c r="G37" s="25" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="H37" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J37" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K37" s="16" t="s">
         <v>10</v>
@@ -3533,13 +3533,13 @@
         <v>33</v>
       </c>
       <c r="G38" s="17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J38" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K38" s="16" t="s">
         <v>10</v>
@@ -3566,22 +3566,22 @@
         <v>34</v>
       </c>
       <c r="G39" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J39" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K39" s="16" t="s">
         <v>10</v>
       </c>
       <c r="L39" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M39" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N39" s="16" t="s">
         <v>8</v>
@@ -3605,13 +3605,13 @@
         <v>35</v>
       </c>
       <c r="G40" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H40" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J40" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K40" s="16" t="s">
         <v>10</v>
@@ -3638,22 +3638,22 @@
         <v>36</v>
       </c>
       <c r="G41" s="27" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="H41" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J41" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K41" s="16" t="s">
         <v>10</v>
       </c>
       <c r="L41" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M41" s="16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N41" s="16" t="s">
         <v>8</v>
@@ -3677,22 +3677,22 @@
         <v>37</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H42" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J42" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K42" s="16" t="s">
         <v>10</v>
       </c>
       <c r="L42" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M42" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N42" s="16" t="s">
         <v>8</v>
@@ -3716,13 +3716,13 @@
         <v>38</v>
       </c>
       <c r="G43" s="27" t="s">
-        <v>282</v>
+        <v>330</v>
       </c>
       <c r="H43" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J43" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K43" s="16" t="s">
         <v>10</v>
@@ -3749,22 +3749,22 @@
         <v>39</v>
       </c>
       <c r="G44" s="23" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H44" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J44" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K44" s="16" t="s">
         <v>10</v>
       </c>
       <c r="L44" s="37" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="M44" s="30" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="N44" s="35">
         <v>40724</v>
@@ -3785,16 +3785,16 @@
         <v>13</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G45" s="23" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="H45" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J45" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K45" s="16" t="s">
         <v>10</v>
@@ -3821,19 +3821,19 @@
         <v>40</v>
       </c>
       <c r="G46" s="17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H46" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J46" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K46" s="16" t="s">
         <v>10</v>
       </c>
       <c r="L46" s="18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M46" s="16" t="s">
         <v>41</v>
@@ -3855,7 +3855,7 @@
         <v>42</v>
       </c>
       <c r="G47" s="17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="N47" s="16" t="s">
         <v>8</v>
@@ -3879,13 +3879,13 @@
         <v>43</v>
       </c>
       <c r="G48" s="17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H48" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J48" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K48" s="16" t="s">
         <v>10</v>
@@ -3907,7 +3907,7 @@
         <v>44</v>
       </c>
       <c r="G49" s="17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N49" s="16" t="s">
         <v>8</v>
@@ -3934,13 +3934,13 @@
         <v>1</v>
       </c>
       <c r="G50" s="23" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H50" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J50" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K50" s="16" t="s">
         <v>10</v>
@@ -3973,10 +3973,10 @@
         <v>46</v>
       </c>
       <c r="H51" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J51" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K51" s="16" t="s">
         <v>10</v>
@@ -3998,7 +3998,7 @@
         <v>47</v>
       </c>
       <c r="G52" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N52" s="16" t="s">
         <v>8</v>
@@ -4022,13 +4022,13 @@
         <v>48</v>
       </c>
       <c r="G53" s="23" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H53" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J53" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K53" s="16" t="s">
         <v>10</v>
@@ -4050,7 +4050,7 @@
         <v>49</v>
       </c>
       <c r="G54" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="N54" s="16" t="s">
         <v>8</v>
@@ -4074,13 +4074,13 @@
         <v>50</v>
       </c>
       <c r="G55" s="17" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H55" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J55" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K55" s="16" t="s">
         <v>10</v>
@@ -4102,7 +4102,7 @@
         <v>51</v>
       </c>
       <c r="G56" s="17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N56" s="16" t="s">
         <v>8</v>
@@ -4126,13 +4126,13 @@
         <v>52</v>
       </c>
       <c r="G57" s="17" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H57" s="16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J57" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K57" s="16" t="s">
         <v>10</v>
@@ -4154,7 +4154,7 @@
         <v>53</v>
       </c>
       <c r="G58" s="17" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N58" s="16" t="s">
         <v>8</v>
@@ -4178,19 +4178,19 @@
         <v>54</v>
       </c>
       <c r="G59" s="23" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H59" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J59" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K59" s="16" t="s">
         <v>10</v>
       </c>
       <c r="L59" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M59" s="16" t="s">
         <v>55</v>
@@ -4214,7 +4214,7 @@
         <v>56</v>
       </c>
       <c r="G60" s="17" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="N60" s="16" t="s">
         <v>8</v>
@@ -4238,13 +4238,13 @@
         <v>57</v>
       </c>
       <c r="G61" s="23" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H61" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J61" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K61" s="16" t="s">
         <v>10</v>
@@ -4266,7 +4266,7 @@
         <v>58</v>
       </c>
       <c r="G62" s="17" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N62" s="16" t="s">
         <v>8</v>
@@ -4290,19 +4290,19 @@
         <v>59</v>
       </c>
       <c r="G63" s="17" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H63" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J63" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K63" s="16" t="s">
         <v>10</v>
       </c>
       <c r="L63" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M63" s="16" t="s">
         <v>60</v>
@@ -4324,7 +4324,7 @@
         <v>61</v>
       </c>
       <c r="G64" s="17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="N64" s="16" t="s">
         <v>8</v>
@@ -4348,13 +4348,13 @@
         <v>62</v>
       </c>
       <c r="G65" s="25" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H65" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J65" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K65" s="16" t="s">
         <v>10</v>
@@ -4383,19 +4383,19 @@
         <v>63</v>
       </c>
       <c r="G66" s="23" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H66" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J66" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K66" s="16" t="s">
         <v>64</v>
       </c>
       <c r="L66" s="18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M66" s="16" t="s">
         <v>65</v>
@@ -4417,7 +4417,7 @@
         <v>66</v>
       </c>
       <c r="G67" s="17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N67" s="16" t="s">
         <v>8</v>
@@ -4444,10 +4444,10 @@
         <v>67</v>
       </c>
       <c r="H68" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J68" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K68" s="16" t="s">
         <v>10</v>
@@ -4469,7 +4469,7 @@
         <v>69</v>
       </c>
       <c r="G69" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N69" s="16" t="s">
         <v>8</v>
@@ -4496,10 +4496,10 @@
         <v>70</v>
       </c>
       <c r="H70" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J70" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K70" s="16" t="s">
         <v>10</v>
@@ -4526,13 +4526,13 @@
         <v>72</v>
       </c>
       <c r="G71" s="17" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H71" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J71" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K71" s="16" t="s">
         <v>10</v>
@@ -4559,13 +4559,13 @@
         <v>73</v>
       </c>
       <c r="G72" s="17" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H72" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J72" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K72" s="16" t="s">
         <v>10</v>
@@ -4592,13 +4592,13 @@
         <v>74</v>
       </c>
       <c r="G73" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H73" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J73" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K73" s="16" t="s">
         <v>10</v>
@@ -4625,13 +4625,13 @@
         <v>75</v>
       </c>
       <c r="G74" s="17" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H74" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J74" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K74" s="16" t="s">
         <v>76</v>
@@ -4653,7 +4653,7 @@
         <v>77</v>
       </c>
       <c r="G75" s="17" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N75" s="16" t="s">
         <v>8</v>
@@ -4677,13 +4677,13 @@
         <v>78</v>
       </c>
       <c r="G76" s="17" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H76" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J76" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K76" s="16" t="s">
         <v>10</v>
@@ -4705,7 +4705,7 @@
         <v>79</v>
       </c>
       <c r="G77" s="17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N77" s="16" t="s">
         <v>8</v>
@@ -4726,16 +4726,16 @@
         <v>79</v>
       </c>
       <c r="E78" s="16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G78" s="17" t="s">
         <v>80</v>
       </c>
       <c r="H78" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J78" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K78" s="16" t="s">
         <v>10</v>
@@ -4757,7 +4757,7 @@
         <v>81</v>
       </c>
       <c r="G79" s="17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N79" s="16" t="s">
         <v>8</v>
@@ -4784,10 +4784,10 @@
         <v>82</v>
       </c>
       <c r="H80" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J80" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K80" s="16" t="s">
         <v>10</v>
@@ -4814,13 +4814,13 @@
         <v>84</v>
       </c>
       <c r="G81" s="17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H81" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J81" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K81" s="16" t="s">
         <v>10</v>
@@ -4842,7 +4842,7 @@
         <v>85</v>
       </c>
       <c r="G82" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N82" s="16" t="s">
         <v>8</v>
@@ -4866,13 +4866,13 @@
         <v>86</v>
       </c>
       <c r="G83" s="27" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H83" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J83" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K83" s="16" t="s">
         <v>10</v>
@@ -4894,7 +4894,7 @@
         <v>87</v>
       </c>
       <c r="G84" s="17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N84" s="16" t="s">
         <v>8</v>
@@ -4918,22 +4918,22 @@
         <v>88</v>
       </c>
       <c r="G85" s="17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H85" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J85" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K85" s="16" t="s">
         <v>10</v>
       </c>
       <c r="L85" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M85" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N85" s="16" t="s">
         <v>8</v>
@@ -4952,7 +4952,7 @@
         <v>89</v>
       </c>
       <c r="G86" s="17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N86" s="16" t="s">
         <v>8</v>
@@ -4976,13 +4976,13 @@
         <v>90</v>
       </c>
       <c r="G87" s="17" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H87" s="16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J87" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K87" s="16" t="s">
         <v>10</v>
@@ -5004,7 +5004,7 @@
         <v>91</v>
       </c>
       <c r="G88" s="17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J88" s="18"/>
       <c r="N88" s="16" t="s">
@@ -5032,10 +5032,10 @@
         <v>92</v>
       </c>
       <c r="H89" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J89" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K89" s="16" t="s">
         <v>10</v>
@@ -5057,7 +5057,7 @@
         <v>94</v>
       </c>
       <c r="G90" s="17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N90" s="16" t="s">
         <v>8</v>
@@ -5084,10 +5084,10 @@
         <v>95</v>
       </c>
       <c r="H91" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J91" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K91" s="16" t="s">
         <v>10</v>
@@ -5095,7 +5095,7 @@
       <c r="N91" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="O91" s="69">
+      <c r="O91" s="61">
         <v>41516</v>
       </c>
     </row>
@@ -5111,7 +5111,7 @@
         <v>97</v>
       </c>
       <c r="G92" s="17" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="N92" s="16" t="s">
         <v>8</v>
@@ -5135,13 +5135,13 @@
         <v>98</v>
       </c>
       <c r="G93" s="17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H93" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J93" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K93" s="16" t="s">
         <v>10</v>
@@ -5163,7 +5163,7 @@
         <v>99</v>
       </c>
       <c r="G94" s="17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="N94" s="16" t="s">
         <v>8</v>
@@ -5187,19 +5187,19 @@
         <v>100</v>
       </c>
       <c r="G95" s="27" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H95" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J95" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K95" s="16" t="s">
         <v>10</v>
       </c>
       <c r="L95" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M95" s="16" t="s">
         <v>101</v>
@@ -5221,7 +5221,7 @@
         <v>102</v>
       </c>
       <c r="G96" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="N96" s="16" t="s">
         <v>8</v>
@@ -5248,10 +5248,10 @@
         <v>103</v>
       </c>
       <c r="H97" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J97" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K97" s="16" t="s">
         <v>10</v>
@@ -5273,7 +5273,7 @@
         <v>105</v>
       </c>
       <c r="G98" s="17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N98" s="16" t="s">
         <v>8</v>
@@ -5297,13 +5297,13 @@
         <v>106</v>
       </c>
       <c r="G99" s="17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H99" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J99" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K99" s="16" t="s">
         <v>10</v>
@@ -5330,13 +5330,13 @@
         <v>107</v>
       </c>
       <c r="G100" s="25" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H100" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J100" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K100" s="16" t="s">
         <v>10</v>
@@ -5358,7 +5358,7 @@
         <v>108</v>
       </c>
       <c r="G101" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N101" s="16" t="s">
         <v>8</v>
@@ -5382,19 +5382,19 @@
         <v>109</v>
       </c>
       <c r="G102" s="23" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H102" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J102" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K102" s="16" t="s">
         <v>10</v>
       </c>
       <c r="L102" s="18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M102" s="28" t="s">
         <v>41</v>
@@ -5418,16 +5418,16 @@
         <v>108</v>
       </c>
       <c r="E103" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="G103" s="17" t="s">
+        <v>331</v>
+      </c>
+      <c r="I103" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="G103" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="I103" s="16" t="s">
-        <v>112</v>
-      </c>
       <c r="J103" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K103" s="16" t="s">
         <v>10</v>
@@ -5451,16 +5451,16 @@
         <v>108</v>
       </c>
       <c r="E104" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G104" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I104" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J104" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K104" s="16" t="s">
         <v>10</v>
@@ -5479,10 +5479,10 @@
       </c>
       <c r="C105" s="33"/>
       <c r="D105" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G105" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="N105" s="16" t="s">
         <v>8</v>
@@ -5500,25 +5500,25 @@
         <v>103</v>
       </c>
       <c r="D106" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="E106" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="E106" s="16" t="s">
-        <v>116</v>
-      </c>
       <c r="G106" s="23" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H106" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J106" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K106" s="16" t="s">
         <v>10</v>
       </c>
       <c r="L106" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M106" s="16" t="s">
         <v>15</v>
@@ -5539,19 +5539,19 @@
         <v>103</v>
       </c>
       <c r="D107" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E107" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="G107" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="I107" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="G107" s="23" t="s">
-        <v>260</v>
-      </c>
-      <c r="I107" s="16" t="s">
-        <v>118</v>
-      </c>
       <c r="J107" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K107" s="16" t="s">
         <v>10</v>
@@ -5572,28 +5572,28 @@
         <v>103</v>
       </c>
       <c r="D108" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E108" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="G108" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="H108" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="J108" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="K108" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L108" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="M108" s="16" t="s">
         <v>120</v>
-      </c>
-      <c r="G108" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="H108" s="16" t="s">
-        <v>214</v>
-      </c>
-      <c r="J108" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="K108" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="L108" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="M108" s="16" t="s">
-        <v>121</v>
       </c>
       <c r="N108" s="16" t="s">
         <v>8</v>
@@ -5609,13 +5609,13 @@
       </c>
       <c r="C109" s="33"/>
       <c r="D109" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G109" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H109" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N109" s="16" t="s">
         <v>8</v>
@@ -5633,19 +5633,19 @@
         <v>107</v>
       </c>
       <c r="D110" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="E110" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="G110" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="E110" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="G110" s="17" t="s">
-        <v>123</v>
-      </c>
       <c r="H110" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J110" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K110" s="16" t="s">
         <v>10</v>
@@ -5664,10 +5664,10 @@
       </c>
       <c r="C111" s="33"/>
       <c r="D111" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G111" s="17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="N111" s="16" t="s">
         <v>8</v>
@@ -5685,19 +5685,19 @@
         <v>109</v>
       </c>
       <c r="D112" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="E112" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G112" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="E112" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="G112" s="17" t="s">
-        <v>126</v>
-      </c>
       <c r="H112" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J112" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K112" s="16" t="s">
         <v>10</v>
@@ -5716,10 +5716,10 @@
       </c>
       <c r="C113" s="33"/>
       <c r="D113" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G113" s="17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="N113" s="16" t="s">
         <v>8</v>
@@ -5737,19 +5737,19 @@
         <v>111</v>
       </c>
       <c r="D114" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="E114" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="E114" s="16" t="s">
-        <v>129</v>
-      </c>
       <c r="G114" s="17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H114" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J114" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K114" s="16" t="s">
         <v>10</v>
@@ -5768,10 +5768,10 @@
       </c>
       <c r="C115" s="33"/>
       <c r="D115" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G115" s="17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="N115" s="16" t="s">
         <v>8</v>
@@ -5789,19 +5789,19 @@
         <v>113</v>
       </c>
       <c r="D116" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="E116" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="E116" s="16" t="s">
-        <v>131</v>
-      </c>
       <c r="G116" s="17" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H116" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J116" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K116" s="16" t="s">
         <v>10</v>
@@ -5820,10 +5820,10 @@
       </c>
       <c r="C117" s="33"/>
       <c r="D117" s="16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G117" s="17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="N117" s="16" t="s">
         <v>8</v>
@@ -5841,25 +5841,25 @@
         <v>115</v>
       </c>
       <c r="D118" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="E118" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="E118" s="16" t="s">
-        <v>133</v>
-      </c>
       <c r="G118" s="17" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H118" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J118" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K118" s="16" t="s">
         <v>10</v>
       </c>
       <c r="L118" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M118" s="16" t="s">
         <v>15</v>
@@ -5880,19 +5880,19 @@
         <v>115</v>
       </c>
       <c r="D119" s="16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E119" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G119" s="23" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H119" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J119" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K119" s="16" t="s">
         <v>10</v>
@@ -5911,10 +5911,10 @@
       </c>
       <c r="C120" s="33"/>
       <c r="D120" s="16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G120" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="N120" s="16" t="s">
         <v>8</v>
@@ -5932,19 +5932,19 @@
         <v>118</v>
       </c>
       <c r="D121" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="E121" s="16" t="s">
+        <v>295</v>
+      </c>
+      <c r="G121" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="E121" s="16" t="s">
-        <v>297</v>
-      </c>
-      <c r="G121" s="17" t="s">
-        <v>136</v>
-      </c>
       <c r="H121" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J121" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K121" s="16" t="s">
         <v>10</v>
@@ -5963,10 +5963,10 @@
       </c>
       <c r="C122" s="33"/>
       <c r="D122" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G122" s="17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="N122" s="16" t="s">
         <v>8</v>
@@ -5984,28 +5984,28 @@
         <v>120</v>
       </c>
       <c r="D123" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="E123" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="E123" s="16" t="s">
-        <v>138</v>
-      </c>
       <c r="G123" s="27" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H123" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J123" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K123" s="16" t="s">
         <v>10</v>
       </c>
       <c r="L123" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="M123" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="N123" s="16" t="s">
         <v>8</v>
@@ -6021,10 +6021,10 @@
       </c>
       <c r="C124" s="33"/>
       <c r="D124" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G124" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="N124" s="16" t="s">
         <v>8</v>
@@ -6042,19 +6042,19 @@
         <v>122</v>
       </c>
       <c r="D125" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="E125" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="G125" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="E125" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="G125" s="17" t="s">
-        <v>140</v>
-      </c>
       <c r="H125" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J125" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K125" s="16" t="s">
         <v>10</v>
@@ -6073,10 +6073,10 @@
       </c>
       <c r="C126" s="33"/>
       <c r="D126" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G126" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="N126" s="16" t="s">
         <v>8</v>
@@ -6094,19 +6094,19 @@
         <v>124</v>
       </c>
       <c r="D127" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="E127" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="E127" s="16" t="s">
-        <v>143</v>
-      </c>
       <c r="G127" s="17" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H127" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J127" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K127" s="16" t="s">
         <v>10</v>
@@ -6127,12 +6127,12 @@
       </c>
       <c r="C128" s="38"/>
       <c r="D128" s="28" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E128" s="28"/>
       <c r="F128" s="28"/>
       <c r="G128" s="25" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="H128" s="28"/>
       <c r="I128" s="28"/>
@@ -6156,21 +6156,21 @@
         <v>126</v>
       </c>
       <c r="D129" s="28" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E129" s="28" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F129" s="28"/>
       <c r="G129" s="25" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H129" s="28" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I129" s="28"/>
       <c r="J129" s="38" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K129" s="28" t="s">
         <v>10</v>
@@ -6196,18 +6196,18 @@
         <v>13</v>
       </c>
       <c r="E130" s="28" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F130" s="28"/>
       <c r="G130" s="44" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="H130" s="28" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I130" s="28"/>
       <c r="J130" s="38" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K130" s="28" t="s">
         <v>10</v>
@@ -6237,14 +6237,14 @@
       </c>
       <c r="F131" s="28"/>
       <c r="G131" s="25" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H131" s="28" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I131" s="28"/>
       <c r="J131" s="38" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K131" s="28" t="s">
         <v>10</v>
@@ -6267,23 +6267,23 @@
         <v>124</v>
       </c>
       <c r="D132" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E132" s="46" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F132" s="28">
         <v>1</v>
       </c>
       <c r="G132" s="25" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="H132" s="28" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I132" s="28"/>
       <c r="J132" s="38" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K132" s="28" t="s">
         <v>10</v>
@@ -6305,23 +6305,23 @@
         <v>124</v>
       </c>
       <c r="D133" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E133" s="46" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F133" s="28">
         <v>2</v>
       </c>
       <c r="G133" s="25" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H133" s="28" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I133" s="28"/>
       <c r="J133" s="38" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K133" s="28" t="s">
         <v>10</v>
@@ -6341,12 +6341,12 @@
       </c>
       <c r="C134" s="46"/>
       <c r="D134" s="46" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E134" s="46"/>
       <c r="F134" s="46"/>
       <c r="G134" s="52" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H134" s="46"/>
       <c r="I134" s="46"/>
@@ -6369,21 +6369,21 @@
         <v>132</v>
       </c>
       <c r="D135" s="46" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E135" s="46" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F135" s="46"/>
       <c r="G135" s="54" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="H135" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I135" s="46"/>
       <c r="J135" s="49" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K135" s="46" t="s">
         <v>10</v>
@@ -6405,21 +6405,21 @@
         <v>132</v>
       </c>
       <c r="D136" s="46" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E136" s="46" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F136" s="46"/>
       <c r="G136" s="54" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="H136" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I136" s="46"/>
       <c r="J136" s="49" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K136" s="46" t="s">
         <v>10</v>
@@ -6444,24 +6444,24 @@
         <v>53</v>
       </c>
       <c r="E137" s="46" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F137" s="46"/>
       <c r="G137" s="54" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="H137" s="46" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I137" s="46"/>
       <c r="J137" s="49" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K137" s="46" t="s">
         <v>10</v>
       </c>
       <c r="L137" s="49" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M137" s="46" t="s">
         <v>55</v>
@@ -6488,14 +6488,14 @@
       </c>
       <c r="F138" s="46"/>
       <c r="G138" s="52" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="H138" s="46" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I138" s="46"/>
       <c r="J138" s="49" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K138" s="46" t="s">
         <v>10</v>
@@ -6517,21 +6517,21 @@
         <v>124</v>
       </c>
       <c r="D139" s="28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E139" s="45" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F139" s="28"/>
       <c r="G139" s="56" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="H139" s="28" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I139" s="28"/>
       <c r="J139" s="38" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K139" s="28" t="s">
         <v>10</v>
@@ -6551,12 +6551,12 @@
       </c>
       <c r="C140" s="28"/>
       <c r="D140" s="45" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E140" s="28"/>
       <c r="F140" s="28"/>
       <c r="G140" s="45" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="H140" s="28"/>
       <c r="I140" s="28"/>
@@ -6580,21 +6580,21 @@
         <v>138</v>
       </c>
       <c r="D141" s="45" t="s">
+        <v>321</v>
+      </c>
+      <c r="E141" s="45" t="s">
         <v>323</v>
-      </c>
-      <c r="E141" s="45" t="s">
-        <v>325</v>
       </c>
       <c r="F141" s="28"/>
       <c r="G141" s="56" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="H141" s="28" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I141" s="28"/>
       <c r="J141" s="38" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K141" s="28" t="s">
         <v>10</v>
@@ -6607,10 +6607,10 @@
       <c r="O141" s="28"/>
     </row>
     <row r="142" spans="1:15">
-      <c r="A142" s="66">
+      <c r="A142" s="58">
         <v>140</v>
       </c>
-      <c r="B142" s="66">
+      <c r="B142" s="58">
         <v>2</v>
       </c>
       <c r="C142" s="33">
@@ -6620,16 +6620,16 @@
         <v>61</v>
       </c>
       <c r="E142" s="16" t="s">
-        <v>328</v>
-      </c>
-      <c r="G142" s="67" t="s">
-        <v>329</v>
+        <v>326</v>
+      </c>
+      <c r="G142" s="59" t="s">
+        <v>327</v>
       </c>
       <c r="H142" s="28" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J142" s="38" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K142" s="28" t="s">
         <v>10</v>
@@ -6639,10 +6639,10 @@
       </c>
     </row>
     <row r="143" spans="1:15">
-      <c r="A143" s="66">
+      <c r="A143" s="58">
         <v>141</v>
       </c>
-      <c r="B143" s="66">
+      <c r="B143" s="58">
         <v>2</v>
       </c>
       <c r="C143" s="33">
@@ -6651,23 +6651,23 @@
       <c r="D143" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E143" s="68" t="s">
-        <v>330</v>
+      <c r="E143" s="60" t="s">
+        <v>328</v>
       </c>
       <c r="G143" s="17" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="H143" s="28" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J143" s="38" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K143" s="28" t="s">
         <v>10</v>
       </c>
       <c r="L143" s="18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M143" s="28" t="s">
         <v>41</v>
@@ -6723,60 +6723,60 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>64</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:4" ht="15.95" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D5" s="6"/>
     </row>
@@ -6788,170 +6788,170 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>60</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>101</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>55</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>65</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="41" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B20" s="42" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C20" s="42"/>
       <c r="D20" s="43" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="44" spans="5:5">

</xml_diff>